<commit_message>
refactor: change to PSA naming
</commit_message>
<xml_diff>
--- a/GRDP.xlsx
+++ b/GRDP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University of the Philippines\4th Year 2nd Sem (4.2) LAST SEM!\CS 199\shock generation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University of the Philippines\4th Year 2nd Sem (4.2) LAST SEM!\CS 199\CGE_Ipopt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDB2D45-D065-4F79-A151-534FFABF6CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65E393E-5F25-40C5-9C0E-E68748061488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{59DE2949-709D-48F8-8353-B73C8C908E9F}"/>
   </bookViews>
@@ -104,46 +104,46 @@
     <t>BARMM</t>
   </si>
   <si>
-    <t>AGR</t>
-  </si>
-  <si>
-    <t>MIN</t>
-  </si>
-  <si>
-    <t>MAN</t>
-  </si>
-  <si>
-    <t>ESW</t>
-  </si>
-  <si>
-    <t>CON</t>
-  </si>
-  <si>
-    <t>WRT</t>
-  </si>
-  <si>
-    <t>TRS</t>
-  </si>
-  <si>
-    <t>AFS</t>
-  </si>
-  <si>
-    <t>INF</t>
-  </si>
-  <si>
-    <t>FIN</t>
-  </si>
-  <si>
-    <t>REA</t>
-  </si>
-  <si>
-    <t>EDU</t>
-  </si>
-  <si>
-    <t>HHS</t>
-  </si>
-  <si>
-    <t>OTH</t>
+    <t>AFF</t>
+  </si>
+  <si>
+    <t>MAQ</t>
+  </si>
+  <si>
+    <t>MFG</t>
+  </si>
+  <si>
+    <t>ESWW</t>
+  </si>
+  <si>
+    <t>CNS</t>
+  </si>
+  <si>
+    <t>TRD</t>
+  </si>
+  <si>
+    <t>TAS</t>
+  </si>
+  <si>
+    <t>AFSA</t>
+  </si>
+  <si>
+    <t>IAC</t>
+  </si>
+  <si>
+    <t>FIA</t>
+  </si>
+  <si>
+    <t>REOD</t>
+  </si>
+  <si>
+    <t>EDUC</t>
+  </si>
+  <si>
+    <t>HHSW</t>
+  </si>
+  <si>
+    <t>OS</t>
   </si>
 </sst>
 </file>
@@ -643,7 +643,7 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+      <selection activeCell="B1" sqref="B1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>